<commit_message>
Added Question Bank for Geometry
</commit_message>
<xml_diff>
--- a/Math/Excel Files/Weakness/Geometry_Weakness.xlsx
+++ b/Math/Excel Files/Weakness/Geometry_Weakness.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\denni\OneDrive\Desktop\Coding\Python\REE_Quiz_Maker\REE-Quiz-Maker\Math\Excel Files\Weakness\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3984BAB1-449F-46C3-ACFB-DDA65449894B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F351BA5-31E8-485E-BC56-F3E4B8606AEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12315" yWindow="0" windowWidth="16590" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gillesania-PS12" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="ExternalData_1" localSheetId="0" hidden="1">'Gillesania-PS12'!$A$1:$E$15</definedName>
+    <definedName name="ExternalData_1" localSheetId="0" hidden="1">'Gillesania-PS12'!$A$1:$E$17</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="77">
   <si>
     <t>Questions</t>
   </si>
@@ -253,6 +253,21 @@
   </si>
   <si>
     <t>Geometry</t>
+  </si>
+  <si>
+    <t>A piece of wire is shaped to enclose a square whose area is 169 sq cm. It is then reshaped to enclose a rectangle whose length is 15 cm. The area of the r ectangle is</t>
+  </si>
+  <si>
+    <t>165 sq cm</t>
+  </si>
+  <si>
+    <t>175 sq cm</t>
+  </si>
+  <si>
+    <t>170 sq cm</t>
+  </si>
+  <si>
+    <t>156 sq cm</t>
   </si>
 </sst>
 </file>
@@ -347,8 +362,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1AB1C94C-CF4D-4D48-9A1C-227387A3A9FD}" name="CSV_Gillesania_PS12_Traingles_Quadrilaterals_Polygons" displayName="CSV_Gillesania_PS12_Traingles_Quadrilaterals_Polygons" ref="A1:G15" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:G15" xr:uid="{1AB1C94C-CF4D-4D48-9A1C-227387A3A9FD}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1AB1C94C-CF4D-4D48-9A1C-227387A3A9FD}" name="CSV_Gillesania_PS12_Traingles_Quadrilaterals_Polygons" displayName="CSV_Gillesania_PS12_Traingles_Quadrilaterals_Polygons" ref="A1:G17" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:G17" xr:uid="{1AB1C94C-CF4D-4D48-9A1C-227387A3A9FD}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{561D7794-5272-4BE3-8622-7622BC7037F6}" uniqueName="1" name="Questions" queryTableFieldId="1" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{DB2E2A7C-07BD-42FC-AB67-AFA396ACEAE9}" uniqueName="2" name="A" queryTableFieldId="2" dataDxfId="5"/>
@@ -625,10 +640,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B492D679-E725-43D7-BBD2-F422BFF7D7BF}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -663,326 +678,358 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" t="s">
         <v>69</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="G5" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" t="s">
         <v>2</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G6" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" t="s">
         <v>29</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" t="s">
         <v>3</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="G7" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="A8" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" t="s">
         <v>33</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" t="s">
         <v>34</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" t="s">
         <v>3</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="G8" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="A9" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" t="s">
         <v>36</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" t="s">
         <v>37</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" t="s">
         <v>38</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F9" t="s">
         <v>4</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="G9" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="A10" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" t="s">
         <v>40</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" t="s">
         <v>41</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" t="s">
         <v>42</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" t="s">
         <v>43</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F10" t="s">
         <v>4</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="G10" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="A11" t="s">
         <v>44</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" t="s">
         <v>45</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" t="s">
         <v>46</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" t="s">
         <v>47</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" t="s">
         <v>48</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F11" t="s">
         <v>4</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="G11" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="A12" t="s">
         <v>49</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" t="s">
         <v>50</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" t="s">
         <v>51</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" t="s">
         <v>52</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" t="s">
         <v>53</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="F12" t="s">
         <v>1</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="G12" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="A13" t="s">
         <v>54</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" t="s">
         <v>55</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" t="s">
         <v>56</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" t="s">
         <v>57</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E13" t="s">
         <v>58</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="F13" t="s">
         <v>4</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="G13" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="A14" t="s">
         <v>59</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" t="s">
         <v>61</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" t="s">
         <v>62</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" t="s">
         <v>63</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E14" t="s">
         <v>64</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="F14" t="s">
         <v>1</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="G14" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="A15" t="s">
         <v>60</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" t="s">
         <v>65</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" t="s">
         <v>66</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15" t="s">
         <v>67</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E15" t="s">
         <v>68</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="F15" t="s">
         <v>2</v>
       </c>
-      <c r="G15" s="1" t="s">
-        <v>71</v>
-      </c>
+      <c r="G15" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>